<commit_message>
Documentos da Sprint atualizados
</commit_message>
<xml_diff>
--- a/Sprint-8/Product Backlog-Burndown.xlsx
+++ b/Sprint-8/Product Backlog-Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Desktop\Sprint-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno\Downloads\adocao11\Sprint-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="161">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -480,6 +480,30 @@
   </si>
   <si>
     <t>Criar Método para Copiar  Arquivo para o Sistema</t>
+  </si>
+  <si>
+    <t>É necessário fazer as atualizações da documentação do software, para que esteja de acordo com o código escrito</t>
+  </si>
+  <si>
+    <t>Os documentos devem estar atualizados para servirem de referência ao código e usabilidade do software</t>
+  </si>
+  <si>
+    <t>Atualizar Levantamento de Requisitos</t>
+  </si>
+  <si>
+    <t>Atualizar Caso de Uso</t>
+  </si>
+  <si>
+    <t>Atualizar Classes de View</t>
+  </si>
+  <si>
+    <t>Atualizar Classes Model</t>
+  </si>
+  <si>
+    <t>Atualizar Classes Controller</t>
+  </si>
+  <si>
+    <t>Atualizar relacionamentos das classes</t>
   </si>
 </sst>
 </file>
@@ -1851,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S101"/>
+  <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:E71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3531,191 +3555,197 @@
       <c r="E72" s="5"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="6"/>
+    <row r="73" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E73" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="F73" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="6"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="5">
+        <v>1</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="F74" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="6"/>
+      <c r="A75" s="28"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" s="5">
+        <v>2</v>
+      </c>
+      <c r="E75" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="F75" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="6"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D76" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E76" s="5">
+        <v>1</v>
+      </c>
+      <c r="F76" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="6"/>
+      <c r="A77" s="28"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="F77" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="6"/>
-    </row>
-    <row r="79" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="25"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D78" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="E78" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="F78" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B80" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D80" s="5">
-        <v>2</v>
-      </c>
-      <c r="E80" s="5">
-        <v>1.67</v>
-      </c>
-      <c r="F80" s="6">
-        <v>5</v>
-      </c>
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
-      <c r="C81" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D81" s="5">
-        <v>2</v>
-      </c>
-      <c r="E81" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="F81" s="6">
-        <v>5</v>
-      </c>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="28"/>
-      <c r="B82" s="28"/>
-      <c r="C82" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D82" s="5">
-        <v>2</v>
-      </c>
-      <c r="E82" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F82" s="6">
-        <v>5</v>
-      </c>
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="29"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D83" s="5">
-        <v>2</v>
-      </c>
-      <c r="E83" s="5">
-        <v>2.8</v>
-      </c>
-      <c r="F83" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>139</v>
-      </c>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="6"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="6"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="6"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -3737,9 +3767,9 @@
       <c r="E92" s="5"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="25" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="B93" s="25"/>
       <c r="C93" s="25"/>
@@ -3748,89 +3778,228 @@
       <c r="F93" s="25"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="6"/>
+      <c r="A94" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D94" s="5">
+        <v>2</v>
+      </c>
+      <c r="E94" s="5">
+        <v>1.67</v>
+      </c>
+      <c r="F94" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="6"/>
+      <c r="A95" s="28"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" s="5">
+        <v>2</v>
+      </c>
+      <c r="E95" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="F95" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="6"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D96" s="5">
+        <v>2</v>
+      </c>
+      <c r="E96" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F96" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="6"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6"/>
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D97" s="5">
+        <v>2</v>
+      </c>
+      <c r="E97" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="F97" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="C98" s="6"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
       <c r="F98" s="6"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
+    <row r="99" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C99" s="6"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="6"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
       <c r="F100" s="6"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="25"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="25"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="6"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="6"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="6"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="6"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="6"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="6"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="A59:A64"/>
+  <mergeCells count="37">
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="A73:A78"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A1:F1"/>
@@ -3844,7 +4013,28 @@
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
     <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="A59:A64"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -4105,15 +4295,15 @@
       </c>
       <c r="J6" s="15">
         <f t="shared" si="1"/>
-        <v>347.65670000000006</v>
+        <v>338.80670000000003</v>
       </c>
       <c r="K6" s="15">
         <f t="shared" si="1"/>
-        <v>347.65670000000006</v>
+        <v>338.80670000000003</v>
       </c>
       <c r="L6" s="15">
         <f t="shared" si="1"/>
-        <v>347.65670000000006</v>
+        <v>338.80670000000003</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
@@ -4223,7 +4413,7 @@
       </c>
       <c r="J9" s="15">
         <f>SUMIF('Product Backlog'!F:F,8,'Product Backlog'!E:E)</f>
-        <v>0</v>
+        <v>8.85</v>
       </c>
       <c r="K9" s="15">
         <f>SUMIF('Product Backlog'!F:F,9,'Product Backlog'!E:E)</f>
@@ -4235,11 +4425,11 @@
       </c>
       <c r="M9" s="15">
         <f>SUM(C9:L9)</f>
-        <v>152.3433</v>
+        <v>161.19329999999999</v>
       </c>
       <c r="N9" s="15">
         <f>M9/10</f>
-        <v>15.23433</v>
+        <v>16.119329999999998</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4254,11 +4444,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -4271,6 +4456,11 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>